<commit_message>
Feat: added input validation to loadEnsembleStructure and respective tests
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model5_dGs.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model5_dGs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="227">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -855,13 +855,13 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.7651821862348"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.2348178137652"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2588,10 +2588,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -2671,63 +2671,63 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.99</v>
+        <v>0.928124943041768</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1.01</v>
+        <v>1.07187505695823</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.928124943041768</v>
+        <v>0.99</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1.07187505695823</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.99</v>
+        <v>0.980758075213057</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1.01</v>
+        <v>1.01924192478694</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.980758075213057</v>
+        <v>0.99</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1.01924192478694</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -2741,35 +2741,35 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.99</v>
+        <v>0.850553653712464</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1.01</v>
+        <v>1.14944634628754</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.850553653712464</v>
+        <v>0.99</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1.14944634628754</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -2783,7 +2783,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -2797,77 +2797,77 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.99</v>
+        <v>0.998343913039016</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1.01</v>
+        <v>1.00165608696098</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0.998343913039016</v>
+        <v>0.925834010503215</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1.00165608696098</v>
+        <v>1.07416598949679</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.925834010503215</v>
+        <v>0.914831185724609</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1.07416598949679</v>
+        <v>1.08516881427539</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.914831185724609</v>
+        <v>0.889197992439507</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>1.08516881427539</v>
+        <v>1.11080200756049</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.889197992439507</v>
+        <v>0.99</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>1.11080200756049</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.99</v>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.99</v>
@@ -2895,77 +2895,77 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0.99</v>
+        <v>0.912928600623706</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>1.01</v>
+        <v>1.08707139937629</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.99</v>
+        <v>0.885298914584682</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>1.01</v>
+        <v>1.11470108541532</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.912928600623706</v>
+        <v>0.99</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>1.08707139937629</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.885298914584682</v>
+        <v>0.99</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>1.11470108541532</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.99</v>
+        <v>0.923333362502783</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>1.01</v>
+        <v>1.07666663749722</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.99</v>
@@ -2979,21 +2979,21 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0.923333362502783</v>
+        <v>0.955157747123127</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>1.07666663749722</v>
+        <v>1.04484225287687</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.99</v>
@@ -3007,77 +3007,77 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0.955157747123127</v>
+        <v>0.824707049979672</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>1.04484225287687</v>
+        <v>1.17529295002033</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0.99</v>
+        <v>0.952987338158675</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>1.01</v>
+        <v>1.04701266184133</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>0.824707049979672</v>
+        <v>0.873263888888888</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>1.17529295002033</v>
+        <v>1.12673611111111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0.952987338158675</v>
+        <v>0.99</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>1.04701266184133</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0.873263888888888</v>
+        <v>0.99</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>1.12673611111111</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0.99</v>
@@ -3091,21 +3091,21 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.99</v>
+        <v>0.944333167529983</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>1.01</v>
+        <v>1.05566683247002</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0.99</v>
@@ -3119,63 +3119,63 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>0.944333167529983</v>
+        <v>0.890748496539046</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>1.05566683247002</v>
+        <v>1.10925150346095</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0.99</v>
+        <v>0.738916363773338</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>1.01</v>
+        <v>1.26108363622666</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0.890748496539046</v>
+        <v>0.99</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>1.10925150346095</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>0.738916363773338</v>
+        <v>0.99</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>1.26108363622666</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0.99</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0.99</v>
@@ -3203,7 +3203,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0.99</v>
@@ -3217,7 +3217,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0.99</v>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0.99</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0.99</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0.99</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0.99</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0.99</v>
@@ -3299,34 +3299,8 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="C51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" s="0" t="n">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>1.01</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3352,9 +3326,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -12323,8 +12297,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>